<commit_message>
Upgrading TP1 to 2024 version
</commit_message>
<xml_diff>
--- a/TP1/cleaning_defib_data.xlsx
+++ b/TP1/cleaning_defib_data.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epfedu-my.sharepoint.com/personal/thalita_drumond_epf_fr/Documents/Teaching/MDE_DataCleaning/data-cleaning-git-repo/TP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_B6EBD7D27A0B55314E5EBB6C360844934EE908D2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5C45F12-BA59-4BD9-8233-E149CECC3B5B}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_B6EBD7D27A0B55314E5EBB6C360844934EE908D2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA5FCBF3-CC44-45CC-A51A-3B412335812D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
     <sheet name="Organizing columns" sheetId="2" r:id="rId2"/>
     <sheet name="Problems in col TEMPLATE" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Problems in column</t>
   </si>
@@ -30,12 +43,6 @@
     <t>Column name:</t>
   </si>
   <si>
-    <t>Formating</t>
-  </si>
-  <si>
-    <t>Sanitizing</t>
-  </si>
-  <si>
     <t>Problem description</t>
   </si>
   <si>
@@ -45,9 +52,6 @@
     <t>What it should be</t>
   </si>
   <si>
-    <t>What it is (after formating)</t>
-  </si>
-  <si>
     <t>Columns to KEEP</t>
   </si>
   <si>
@@ -211,6 +215,12 @@
   </si>
   <si>
     <t>chgtpiles</t>
+  </si>
+  <si>
+    <t>Keep/Drop/Merge?</t>
+  </si>
+  <si>
+    <t>Appropriate Format (data type) in pandas</t>
   </si>
 </sst>
 </file>
@@ -294,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -323,11 +333,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -341,10 +358,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Columns" displayName="Columns" ref="A1:A52" totalsRowShown="0">
-  <autoFilter ref="A1:A52" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ColumnInfo" displayName="ColumnInfo" ref="A1:C52" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C52" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colum names"/>
+    <tableColumn id="2" xr3:uid="{D1D04763-36BC-40D1-8289-078EB9DCEBCB}" name="Keep/Drop/Merge?"/>
+    <tableColumn id="3" xr3:uid="{C6717A7C-5D54-472C-AAC0-289BF1AB7031}" name="Appropriate Format (data type) in pandas"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -369,18 +388,6 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Problem description"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="What it is"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="What it should be"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table4" displayName="Table4" ref="E5:G31" totalsRowShown="0">
-  <autoFilter ref="E5:G31" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Problem description"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="What it is (after formating)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="What it should be"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -674,278 +681,298 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A52"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="21" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="22" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="23" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="24" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="25" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="26" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="27" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="28" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="29" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="30" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="31" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="32" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="33" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="34" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="35" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="36" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="37" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="38" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="39" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="40" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="41" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="42" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="43" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="44" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="45" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="46" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="47" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="48" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="49" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="50" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="51" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="52" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>62</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B52" xr:uid="{E5A0C742-7A43-400A-B35D-002A11DBC128}">
+      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="x12ac">
+          <x12ac:list>"""keep"", ""drop"", ""merge"""</x12ac:list>
+        </mc:Choice>
+        <mc:Fallback>
+          <formula1>"""keep"", ""drop"", ""merge"""</formula1>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -960,196 +987,198 @@
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
     </row>
-    <row r="33" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
     </row>
-    <row r="34" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
     </row>
-    <row r="35" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1159,6 +1188,18 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6E248C7F-2965-4B22-9988-8D941F92B75C}">
+          <x14:formula1>
+            <xm:f>Columns!A2:A52</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:C36</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1169,64 +1210,56 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1235,7 +1268,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1244,7 +1277,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1253,7 +1286,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1262,7 +1295,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1271,7 +1304,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1280,7 +1313,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1289,7 +1322,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1298,7 +1331,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1307,7 +1340,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1316,7 +1349,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1325,7 +1358,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1334,7 +1367,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1343,7 +1376,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1352,7 +1385,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1361,7 +1394,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1370,7 +1403,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1379,7 +1412,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1388,7 +1421,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1397,7 +1430,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1406,7 +1439,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1415,7 +1448,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1424,7 +1457,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1433,7 +1466,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1442,7 +1475,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1451,7 +1484,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1466,9 +1499,20 @@
     <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4CDDC96-33F5-45F8-AA45-904F91147764}">
+          <x14:formula1>
+            <xm:f>Columns!$A$2:$A$52</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>